<commit_message>
basis lijkt redelijk te werken
</commit_message>
<xml_diff>
--- a/basedirs.xlsx
+++ b/basedirs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aapa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98AED7D-717F-4C16-A863-15F6B7E76507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E86507-8E15-466D-91C3-E3723DF385DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D83F1DE4-0F44-441F-831B-31076F4ABD65}"/>
   </bookViews>
@@ -101,7 +101,7 @@
     <t xml:space="preserve"> :ONEDRIVE:\NHL Stenden\HBO-ICT Afstuderen - Software Engineering\2023-2024 </t>
   </si>
   <si>
-    <t>d:\aapa\DEMO\AANVRAGEN</t>
+    <t>d:\aapaDEMO\AANVRAGEN</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
import excel met mapper
</commit_message>
<xml_diff>
--- a/basedirs.xlsx
+++ b/basedirs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aapa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E86507-8E15-466D-91C3-E3723DF385DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEC0612-EAB1-4AF7-BC3C-951EA53AD273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D83F1DE4-0F44-441F-831B-31076F4ABD65}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{D83F1DE4-0F44-441F-831B-31076F4ABD65}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>periode</t>
   </si>
   <si>
-    <t>forms_version</t>
-  </si>
-  <si>
     <t>directory</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>d:\aapaDEMO\AANVRAGEN</t>
+  </si>
+  <si>
+    <t>forms_versie</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,10 +473,10 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -490,7 +490,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -504,7 +504,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -518,7 +518,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -532,7 +532,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -546,7 +546,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -560,7 +560,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -574,7 +574,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -588,7 +588,7 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -602,7 +602,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -616,7 +616,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -630,7 +630,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -644,7 +644,7 @@
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -658,7 +658,7 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>